<commit_message>
Update get_reply function for replacing the username
</commit_message>
<xml_diff>
--- a/Chatbot/Data/replies.xlsx
+++ b/Chatbot/Data/replies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LICENTA\AI-based-solution-for-mental-health-issues\Chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37213CEE-24D8-4B23-85C5-4EF4D0747403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A2369-E597-48C9-BFB7-6845B2EAEAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="10073" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Now, what about you? What's your name?</t>
   </si>
   <si>
-    <t>I am here for you. Together we can pass over it, ok?</t>
-  </si>
-  <si>
     <t>I assume that this feeling can impact your daily activities 🥺</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>If you need something, do not forget to contact me or our amazing team!</t>
+  </si>
+  <si>
+    <t>I am here for you, USER_NAME. Together we can pass over it, ok?</t>
   </si>
 </sst>
 </file>
@@ -503,13 +503,13 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="121.9375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.29296875" customWidth="1"/>
+    <col min="2" max="2" width="62.1171875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.52734375" customWidth="1"/>
     <col min="4" max="4" width="104.8203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59.64453125" bestFit="1" customWidth="1"/>
@@ -524,16 +524,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
@@ -541,19 +541,19 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
@@ -561,19 +561,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -581,19 +581,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
@@ -601,16 +601,16 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
@@ -618,16 +618,16 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
@@ -635,68 +635,68 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sadness functionality completely done
</commit_message>
<xml_diff>
--- a/Chatbot/Data/replies.xlsx
+++ b/Chatbot/Data/replies.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LICENTA\AI-based-solution-for-mental-health-issues\Chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A2369-E597-48C9-BFB7-6845B2EAEAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{782DE167-905B-4AE7-BA31-A676B2B450C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="replies" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>intro</t>
   </si>
@@ -60,21 +60,12 @@
     <t>goodbye</t>
   </si>
   <si>
-    <t>Ok, I am more than happy to see that you found something that can improve your mood ❤</t>
-  </si>
-  <si>
     <t>Until next time, take care of yourself 🤗</t>
   </si>
   <si>
-    <t>Have a wonderful day! 🌸</t>
-  </si>
-  <si>
     <t>We are available at any time of the day.</t>
   </si>
   <si>
-    <t>Now, I would like to do a little exercise with you.</t>
-  </si>
-  <si>
     <t>In medical terms, it is called Thought Record.</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>Sounds interesting, right? 😊</t>
   </si>
   <si>
-    <t>Then let's see the steps that we have to check in order to achieve this new skill! ✨</t>
-  </si>
-  <si>
     <t>As a little tip, you might feel the need to grab a pen and a piece of paper near you</t>
   </si>
   <si>
@@ -123,33 +111,18 @@
     <t>Question 1: What is the effect of believing this thought?</t>
   </si>
   <si>
-    <t>Question 2: What would happen if I didn’t believe this thought?</t>
-  </si>
-  <si>
     <t>Question 3: What is the evidence supporting this thought?</t>
   </si>
   <si>
     <t>Question 4: What is the evidence against this thought?</t>
   </si>
   <si>
-    <t>Question 5: What’s the worst that could happen, and would I survive it?</t>
-  </si>
-  <si>
     <t>Question 6: What’s the best that could happen?</t>
   </si>
   <si>
     <t>Question 7: What is the most likely?</t>
   </si>
   <si>
-    <t>Question 8: If my friend was in this situation, what would I tell him/her?</t>
-  </si>
-  <si>
-    <t>Question 9: What can I do about this?</t>
-  </si>
-  <si>
-    <t>It seems that this solution doesn't help you enough…</t>
-  </si>
-  <si>
     <t>I am sorry to see that…</t>
   </si>
   <si>
@@ -172,6 +145,81 @@
   </si>
   <si>
     <t>I am here for you, USER_NAME. Together we can pass over it, ok?</t>
+  </si>
+  <si>
+    <t>Ok, USER_NAME, I am more than happy to see that you found something that can improve your mood ❤</t>
+  </si>
+  <si>
+    <t>Have a wonderful day, USER_NAME! 🌸</t>
+  </si>
+  <si>
+    <t>Now, I would like to do a little exercise with you, USER_NAME.</t>
+  </si>
+  <si>
+    <t>It seems that this solution doesn't help you enough, USER_NAME…</t>
+  </si>
+  <si>
+    <t>Then let's see the steps that we have to check in order to achieve this new skill, USER_NAME! ✨</t>
+  </si>
+  <si>
+    <t>In general, it takes between 1 and 3 minutes to complete them, but I encourage you to take your time and reflect ✨</t>
+  </si>
+  <si>
+    <t>I know that this activity can be emotionally consuming, so just type READY when you finish 😊</t>
+  </si>
+  <si>
+    <t>Now I will let you do the steps from 1 to 3, USER_NAME.</t>
+  </si>
+  <si>
+    <t>find_automatic_thought</t>
+  </si>
+  <si>
+    <t>Ok, USER_NAME, now that you completed the steps from 1 to 3, let's move forward! ✨</t>
+  </si>
+  <si>
+    <t>Please pick one automatic thought from your list</t>
+  </si>
+  <si>
+    <t>Considering it, you should respond to the following questions</t>
+  </si>
+  <si>
+    <t>Question 2: What would happen if you didn’t believe this thought?</t>
+  </si>
+  <si>
+    <t>Question 5: What’s the worst that could happen, and would you survive it?</t>
+  </si>
+  <si>
+    <t>Question 8: If your friend was in this situation, what would you tell him/her?</t>
+  </si>
+  <si>
+    <t>Question 9: What can you do about this?</t>
+  </si>
+  <si>
+    <t>Now, USER_NAME, use your responses to these questions to create an alternative response</t>
+  </si>
+  <si>
+    <t>This answer could be used for defending the automatic thought that may cause your negative emotion</t>
+  </si>
+  <si>
+    <t>When you are ready, please let me know what idea you developed 🤗</t>
+  </si>
+  <si>
+    <t>find_alternative_response</t>
+  </si>
+  <si>
+    <t>congratulations</t>
+  </si>
+  <si>
+    <t>Good job, USER_NAME! 🎉</t>
+  </si>
+  <si>
+    <t>I am more than happy to see that you succeed in reconstructing the way in which you think!</t>
+  </si>
+  <si>
+    <t>Don't forget to apply this exercise every time to feel overwhelmed by a thought.</t>
+  </si>
+  <si>
+    <t>So, USER_NAME, what automatic thought bothers you the most? 💫</t>
   </si>
 </sst>
 </file>
@@ -500,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -512,11 +560,14 @@
     <col min="2" max="2" width="62.1171875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.52734375" customWidth="1"/>
     <col min="4" max="4" width="104.8203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.64453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.17578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="104.8203125" customWidth="1"/>
+    <col min="6" max="6" width="59.64453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.17578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.64453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.3515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,36 +578,54 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -564,19 +633,28 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -584,119 +662,148 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.5">
+      <c r="D17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="D13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="D14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="D15" t="s">
-        <v>26</v>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.5">
+      <c r="D18" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Web app + reformat code
</commit_message>
<xml_diff>
--- a/Chatbot/Data/replies.xlsx
+++ b/Chatbot/Data/replies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LICENTA\AI-based-solution-for-mental-health-issues\Chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{782DE167-905B-4AE7-BA31-A676B2B450C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D82BD3D-FEF8-46B4-AA8C-25672DAA0A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3940" yWindow="2907" windowWidth="19200" windowHeight="10073" tabRatio="377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="replies" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
   <si>
     <t>intro</t>
   </si>
@@ -84,24 +84,9 @@
     <t>Sounds interesting, right? 😊</t>
   </si>
   <si>
-    <t>As a little tip, you might feel the need to grab a pen and a piece of paper near you</t>
-  </si>
-  <si>
     <t>Step 1: Identify the situation that triggered the negative emotion that you feel right now 🌪️</t>
   </si>
   <si>
-    <t>Step 2: Write down the emotions that triggered because of the situation. Rate their intensity from 0 to 10 💫</t>
-  </si>
-  <si>
-    <t>Step 5: Using your answers to the probing questions, develop a short alternative response to the automatic thought you choose 🌞</t>
-  </si>
-  <si>
-    <t>Step 4: Choose the automatic thought that is most responsible for your distress, and use it to answer the probing questions 🌤️</t>
-  </si>
-  <si>
-    <t>Step 3: List all of your automatic thoughts that came in your mind and rate how much you believe them on a scale from 0-10 ☘️</t>
-  </si>
-  <si>
     <t>thought_record_probing_questions</t>
   </si>
   <si>
@@ -144,9 +129,6 @@
     <t>If you need something, do not forget to contact me or our amazing team!</t>
   </si>
   <si>
-    <t>I am here for you, USER_NAME. Together we can pass over it, ok?</t>
-  </si>
-  <si>
     <t>Ok, USER_NAME, I am more than happy to see that you found something that can improve your mood ❤</t>
   </si>
   <si>
@@ -159,27 +141,15 @@
     <t>It seems that this solution doesn't help you enough, USER_NAME…</t>
   </si>
   <si>
-    <t>Then let's see the steps that we have to check in order to achieve this new skill, USER_NAME! ✨</t>
-  </si>
-  <si>
-    <t>In general, it takes between 1 and 3 minutes to complete them, but I encourage you to take your time and reflect ✨</t>
-  </si>
-  <si>
     <t>I know that this activity can be emotionally consuming, so just type READY when you finish 😊</t>
   </si>
   <si>
-    <t>Now I will let you do the steps from 1 to 3, USER_NAME.</t>
-  </si>
-  <si>
     <t>find_automatic_thought</t>
   </si>
   <si>
     <t>Ok, USER_NAME, now that you completed the steps from 1 to 3, let's move forward! ✨</t>
   </si>
   <si>
-    <t>Please pick one automatic thought from your list</t>
-  </si>
-  <si>
     <t>Considering it, you should respond to the following questions</t>
   </si>
   <si>
@@ -220,6 +190,51 @@
   </si>
   <si>
     <t>So, USER_NAME, what automatic thought bothers you the most? 💫</t>
+  </si>
+  <si>
+    <t>I am here for you, USER_NAME.</t>
+  </si>
+  <si>
+    <t>What usually helps you feel better in this kind of situation, USER_NAME?</t>
+  </si>
+  <si>
+    <t>determine_if_feel_better_action</t>
+  </si>
+  <si>
+    <t>Please respond by YES or NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I see. Do you think there is a way in which you could achieve this right now, USER_NAME? </t>
+  </si>
+  <si>
+    <t>thought_record_details</t>
+  </si>
+  <si>
+    <t>It's alright, don't get scared. In the next moments, we will find other solutions in order to make you feel better ❤</t>
+  </si>
+  <si>
+    <t>thought_record_steps</t>
+  </si>
+  <si>
+    <t>Then let's see the steps that we have to check in order to achieve this skill, USER_NAME! ✨</t>
+  </si>
+  <si>
+    <t>Have you heard of this exercise before, USER_NAME?</t>
+  </si>
+  <si>
+    <t>Step 3: List all of your automatic thoughts that came in your mind ☘️</t>
+  </si>
+  <si>
+    <t>Choose the automatic thought that is most responsible for your distress</t>
+  </si>
+  <si>
+    <t>Now I will let you complete these steps, USER_NAME.</t>
+  </si>
+  <si>
+    <t>Step 2: Write down the emotions that triggered because of the situation.</t>
+  </si>
+  <si>
+    <t>As a little tip, you might feel the need to grab a pen and a piece of paper near you.</t>
   </si>
 </sst>
 </file>
@@ -548,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -560,14 +575,17 @@
     <col min="2" max="2" width="62.1171875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.52734375" customWidth="1"/>
     <col min="4" max="4" width="104.8203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="104.8203125" customWidth="1"/>
-    <col min="6" max="6" width="59.64453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.17578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.64453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73.3515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101.05859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="104.8203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="104.8203125" customWidth="1"/>
+    <col min="8" max="8" width="59.64453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.87890625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="77.64453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="73.3515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.05859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,54 +596,72 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -633,28 +669,37 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -665,146 +710,126 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="F8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D9" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H9" t="s">
         <v>44</v>
       </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="D13" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D14" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.5">
-      <c r="D17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.5">
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minimal front + sadness&anger scenarios
</commit_message>
<xml_diff>
--- a/Chatbot/Data/replies.xlsx
+++ b/Chatbot/Data/replies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LICENTA\AI-based-solution-for-mental-health-issues\Chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D82BD3D-FEF8-46B4-AA8C-25672DAA0A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B752B8A4-28F7-4B4B-98A4-7F7C388E21FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="2907" windowWidth="19200" windowHeight="10073" tabRatio="377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="2087" windowWidth="19200" windowHeight="10073" tabRatio="377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="replies" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>intro</t>
   </si>
@@ -186,9 +186,6 @@
     <t>I am more than happy to see that you succeed in reconstructing the way in which you think!</t>
   </si>
   <si>
-    <t>Don't forget to apply this exercise every time to feel overwhelmed by a thought.</t>
-  </si>
-  <si>
     <t>So, USER_NAME, what automatic thought bothers you the most? 💫</t>
   </si>
   <si>
@@ -235,6 +232,24 @@
   </si>
   <si>
     <t>As a little tip, you might feel the need to grab a pen and a piece of paper near you.</t>
+  </si>
+  <si>
+    <t>thought_record_knew_exercise</t>
+  </si>
+  <si>
+    <t>Alright, USER_NAME! So let's start the exercise, ok?</t>
+  </si>
+  <si>
+    <t>Don't forget to apply this exercise every time to feel overwhelmed by a thought, ok?</t>
+  </si>
+  <si>
+    <t>handle_anger</t>
+  </si>
+  <si>
+    <t>I can understand this, USER_NAME.</t>
+  </si>
+  <si>
+    <t>I assume that this feeling generates uncomfortable behaviour 🥺</t>
   </si>
 </sst>
 </file>
@@ -563,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -576,16 +591,18 @@
     <col min="3" max="3" width="73.52734375" customWidth="1"/>
     <col min="4" max="4" width="104.8203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="101.05859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="104.8203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="104.8203125" customWidth="1"/>
-    <col min="8" max="8" width="59.64453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.87890625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="77.64453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="73.3515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61.05859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="101.05859375" customWidth="1"/>
+    <col min="7" max="7" width="104.8203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="104.8203125" customWidth="1"/>
+    <col min="9" max="9" width="59.64453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="81.87890625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="77.64453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="73.3515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="72.1171875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="62.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,69 +616,81 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>46</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>51</v>
       </c>
-      <c r="L2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -677,29 +706,32 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>47</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>52</v>
       </c>
-      <c r="L3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -715,31 +747,34 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>41</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -750,20 +785,26 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>68</v>
-      </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -771,65 +812,70 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="F8" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="G8" t="s">
         <v>38</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="H9" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="I9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="H10" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="I10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:14" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>